<commit_message>
updated calculator to only compute risk for age range of dev sample
</commit_message>
<xml_diff>
--- a/results/UKB-DRS_Calculator.xlsx
+++ b/results/UKB-DRS_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melisanaturk/Documents/Oxford_DPhil/Biobank_Analyses/Dementia_risk_project/Manuscript/Supplementary_Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="13_ncr:1_{E0E1620A-CAD1-4949-B6AD-E8FF5CE4AED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B94F7CE8-14FA-4412-839B-D60FDF45640D}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{E0E1620A-CAD1-4949-B6AD-E8FF5CE4AED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{628A3C18-7AF6-4220-BF2F-ACF596C47519}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="460" windowWidth="23460" windowHeight="14580" activeTab="1" xr2:uid="{6004D5AF-BE6E-984F-901F-4E7FEE085423}"/>
+    <workbookView xWindow="1580" yWindow="460" windowWidth="23460" windowHeight="14580" xr2:uid="{6004D5AF-BE6E-984F-901F-4E7FEE085423}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1448,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95B3D4D-1122-414D-9CB5-4AB9572A3F02}">
   <dimension ref="B1:Z1442"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:F32"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -10197,19 +10197,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF4EB25-9C80-B547-9443-AA4112D5F036}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G1048576"/>
+    <sheetView topLeftCell="H1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="25.625" style="16" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="28" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="21.125" style="15" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="17.125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="27" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="35" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="11" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="28" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="17.125" customWidth="1"/>
+    <col min="5" max="5" width="27" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="16383" width="11" customWidth="1"/>
     <col min="16384" max="16384" width="8" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10804,7 +10804,7 @@
       </c>
       <c r="E43" s="50"/>
       <c r="F43" s="28" t="e">
-        <f>F40*100</f>
+        <f>IF(AND(Main!D4&gt;=50,Main!D4 &lt;=73),F40*100,"NA")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10814,7 +10814,7 @@
       </c>
       <c r="E44" s="50"/>
       <c r="F44" s="28">
-        <f>F41*100</f>
+        <f>IF(AND(Main!D4&gt;=50,Main!D4 &lt;=73),F41*100,"NA")</f>
         <v>3.9120965541546253</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated calculator with new model
</commit_message>
<xml_diff>
--- a/results/UKB-DRS_Calculator.xlsx
+++ b/results/UKB-DRS_Calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melisanaturk/Documents/Oxford_DPhil/Biobank_Analyses/Dementia_risk_project/Manuscript/Supplementary_Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{E0E1620A-CAD1-4949-B6AD-E8FF5CE4AED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{628A3C18-7AF6-4220-BF2F-ACF596C47519}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D8A7F66-243B-4A91-B0E5-77007E90C495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="460" windowWidth="23460" windowHeight="14580" xr2:uid="{6004D5AF-BE6E-984F-901F-4E7FEE085423}"/>
+    <workbookView xWindow="1580" yWindow="460" windowWidth="23460" windowHeight="14580" activeTab="1" xr2:uid="{6004D5AF-BE6E-984F-901F-4E7FEE085423}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -68,16 +69,13 @@
     <t>History of Stroke or Transient Ischaemic Stroke:</t>
   </si>
   <si>
-    <t>Use of Antihypertensive medication:</t>
+    <t>Hypertensive:</t>
   </si>
   <si>
-    <t>Use of Aspirin:</t>
+    <t>High Cholesterol:</t>
   </si>
   <si>
     <t>APOE4 carrier:</t>
-  </si>
-  <si>
-    <t>Unknown</t>
   </si>
   <si>
     <t>If APOE information is unavailable, please select "unknown".</t>
@@ -137,13 +135,16 @@
     <t>Stroke/ TIA</t>
   </si>
   <si>
-    <t>Use of Antihypertensives</t>
+    <t>Hypertensive</t>
   </si>
   <si>
-    <t>Use of Aspirin</t>
+    <t>High Cholesterol</t>
   </si>
   <si>
     <t>APOE4 carrier</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
   <si>
     <t>UKBDRS-APOE sum of coefficients:</t>
@@ -558,6 +559,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -576,7 +578,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1448,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95B3D4D-1122-414D-9CB5-4AB9572A3F02}">
   <dimension ref="B1:Z1442"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -1464,13 +1465,13 @@
   <sheetData>
     <row r="1" spans="2:8" hidden="1"/>
     <row r="2" spans="2:8" ht="69.95" customHeight="1">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="2:8" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="C3" s="3"/>
@@ -1483,7 +1484,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="23">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="2:8" s="2" customFormat="1" ht="17.100000000000001" thickBot="1">
@@ -1617,14 +1618,14 @@
         <v>12</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E22" s="19"/>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="2:6" s="2" customFormat="1">
       <c r="C23" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="4"/>
@@ -1637,42 +1638,42 @@
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="2:6" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="2:6" s="2" customFormat="1" ht="17.100000000000001" thickBot="1">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="50"/>
+      <c r="D26" s="20">
+        <f>Hidden!F43</f>
+        <v>5.6883741428118997</v>
+      </c>
+      <c r="E26" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="49"/>
-      <c r="D26" s="20" t="e">
-        <f>Hidden!F43</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E26" s="22" t="s">
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="2:6" s="2" customFormat="1" ht="12" customHeight="1" thickBot="1">
+      <c r="C27" s="48"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="2:6" s="2" customFormat="1" ht="17.100000000000001" thickBot="1">
+      <c r="B28" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="2:6" s="2" customFormat="1" ht="12" customHeight="1" thickBot="1">
-      <c r="C27" s="47"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="2:6" s="2" customFormat="1" ht="17.100000000000001" thickBot="1">
-      <c r="B28" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="49"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="21">
         <f>Hidden!F44</f>
-        <v>3.9120965541546253</v>
+        <v>8.9072716344553484</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F28" s="4"/>
     </row>
@@ -10195,42 +10196,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF4EB25-9C80-B547-9443-AA4112D5F036}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="F1" sqref="B1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="25.625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="28" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="17.125" customWidth="1"/>
-    <col min="5" max="5" width="27" style="1" customWidth="1"/>
-    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="2" max="2" width="28" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.125" style="15" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="17.125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="27" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="35" hidden="1" customWidth="1"/>
     <col min="7" max="16383" width="11" customWidth="1"/>
     <col min="16384" max="16384" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="C1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="D1" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="E1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="35" t="s">
         <v>22</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -10243,42 +10244,42 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="C3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>26</v>
-      </c>
       <c r="D3" s="28">
-        <v>0.18861</v>
+        <v>0.18906000000000001</v>
       </c>
       <c r="E3" s="29">
         <f>Main!D4</f>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F3" s="38">
         <f>D3*E3</f>
-        <v>11.316599999999999</v>
+        <v>12.2889</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="36"/>
       <c r="B4" s="26"/>
       <c r="C4" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="30">
-        <v>0.17968000000000001</v>
+        <v>0.17974999999999999</v>
       </c>
       <c r="E4" s="29">
         <f>Main!D4</f>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F4" s="38">
         <f t="shared" ref="F4:F30" si="0">D4*E4</f>
-        <v>10.780800000000001</v>
+        <v>11.68375</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -10291,16 +10292,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="28">
-        <v>0.28603000000000001</v>
+        <v>0.28544000000000003</v>
       </c>
       <c r="E6" s="29">
         <f>IF(Main!D6="Yes",1,0)</f>
@@ -10308,7 +10309,7 @@
       </c>
       <c r="F6" s="38">
         <f t="shared" ref="F6:F7" si="1">D6*E6</f>
-        <v>0.28603000000000001</v>
+        <v>0.28544000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -10317,10 +10318,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="30">
-        <v>0.41322999999999999</v>
+        <v>0.41210999999999998</v>
       </c>
       <c r="E7" s="29">
         <f>IF(Main!D6="Yes",1,0)</f>
@@ -10328,7 +10329,7 @@
       </c>
       <c r="F7" s="38">
         <f t="shared" si="1"/>
-        <v>0.41322999999999999</v>
+        <v>0.41210999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -10341,16 +10342,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>26</v>
-      </c>
       <c r="D9" s="28">
-        <v>-3.9469999999999998E-2</v>
+        <v>-3.9019999999999999E-2</v>
       </c>
       <c r="E9" s="29">
         <f>Main!D8</f>
@@ -10358,17 +10359,17 @@
       </c>
       <c r="F9" s="38">
         <f t="shared" si="0"/>
-        <v>-0.9867499999999999</v>
+        <v>-0.97550000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="36"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="30">
-        <v>-4.4400000000000002E-2</v>
+        <v>-4.3830000000000001E-2</v>
       </c>
       <c r="E10" s="29">
         <f>Main!D8</f>
@@ -10376,7 +10377,7 @@
       </c>
       <c r="F10" s="38">
         <f t="shared" si="0"/>
-        <v>-1.1100000000000001</v>
+        <v>-1.09575</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -10395,10 +10396,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="30">
-        <v>0.28072999999999998</v>
+        <v>0.27701999999999999</v>
       </c>
       <c r="E12" s="29">
         <f>IF(Main!D10="Yes",1,0)</f>
@@ -10406,7 +10407,7 @@
       </c>
       <c r="F12" s="38">
         <f t="shared" si="0"/>
-        <v>0.28072999999999998</v>
+        <v>0.27701999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75">
@@ -10415,10 +10416,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="30">
-        <v>0.24928</v>
+        <v>0.24526999999999999</v>
       </c>
       <c r="E13" s="29">
         <f>IF(Main!D10="Yes",1,0)</f>
@@ -10426,7 +10427,7 @@
       </c>
       <c r="F13" s="38">
         <f t="shared" si="0"/>
-        <v>0.24928</v>
+        <v>0.24526999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -10439,16 +10440,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="28">
-        <v>0.53912000000000004</v>
+        <v>0.54844999999999999</v>
       </c>
       <c r="E15" s="29">
         <f>IF(Main!D12="Yes",1,0)</f>
@@ -10465,10 +10466,10 @@
         <v>7</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="30">
-        <v>0.55652999999999997</v>
+        <v>0.54864999999999997</v>
       </c>
       <c r="E16" s="29">
         <f>IF(Main!D12="Yes",1,0)</f>
@@ -10489,16 +10490,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="28">
-        <v>0.54122999999999999</v>
+        <v>0.53649999999999998</v>
       </c>
       <c r="E18" s="29">
         <f>IF(Main!D14="Yes",1,0)</f>
@@ -10506,7 +10507,7 @@
       </c>
       <c r="F18" s="38">
         <f t="shared" si="0"/>
-        <v>0.54122999999999999</v>
+        <v>0.53649999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -10515,10 +10516,10 @@
         <v>7</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="30">
-        <v>0.53730999999999995</v>
+        <v>0.53176999999999996</v>
       </c>
       <c r="E19" s="29">
         <f>IF(Main!D14="Yes",1,0)</f>
@@ -10526,7 +10527,7 @@
       </c>
       <c r="F19" s="38">
         <f t="shared" si="0"/>
-        <v>0.53730999999999995</v>
+        <v>0.53176999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -10539,16 +10540,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="28">
-        <v>0.65547999999999995</v>
+        <v>0.68576999999999999</v>
       </c>
       <c r="E21" s="29">
         <f>IF(Main!D16="Yes",1,0)</f>
@@ -10556,7 +10557,7 @@
       </c>
       <c r="F21" s="38">
         <f t="shared" si="0"/>
-        <v>0.65547999999999995</v>
+        <v>0.68576999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -10565,10 +10566,10 @@
         <v>7</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" s="30">
-        <v>0.66173999999999999</v>
+        <v>0.68223999999999996</v>
       </c>
       <c r="E22" s="29">
         <f>IF(Main!D16="Yes",1,0)</f>
@@ -10576,7 +10577,7 @@
       </c>
       <c r="F22" s="38">
         <f t="shared" si="0"/>
-        <v>0.66173999999999999</v>
+        <v>0.68223999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -10589,16 +10590,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" s="28">
-        <v>0.14174</v>
+        <v>0.20688999999999999</v>
       </c>
       <c r="E24" s="29">
         <f>IF(Main!D18="Yes",1,0)</f>
@@ -10606,7 +10607,7 @@
       </c>
       <c r="F24" s="38">
         <f t="shared" si="0"/>
-        <v>0.14174</v>
+        <v>0.20688999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -10615,10 +10616,10 @@
         <v>7</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="30">
-        <v>0.14602999999999999</v>
+        <v>0.17816000000000001</v>
       </c>
       <c r="E25" s="29">
         <f>IF(Main!D18="Yes",1,0)</f>
@@ -10626,7 +10627,7 @@
       </c>
       <c r="F25" s="38">
         <f t="shared" si="0"/>
-        <v>0.14602999999999999</v>
+        <v>0.17816000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17.100000000000001">
@@ -10639,16 +10640,16 @@
     </row>
     <row r="27" spans="1:6" ht="15.75">
       <c r="A27" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="28">
-        <v>0.14349000000000001</v>
+        <v>4.0289999999999999E-2</v>
       </c>
       <c r="E27" s="29">
         <f>IF(Main!D20="Yes",1,0)</f>
@@ -10656,7 +10657,7 @@
       </c>
       <c r="F27" s="38">
         <f t="shared" si="0"/>
-        <v>0.14349000000000001</v>
+        <v>4.0289999999999999E-2</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75">
@@ -10665,10 +10666,10 @@
         <v>7</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="28">
-        <v>0.17352000000000001</v>
+        <v>0.12330000000000001</v>
       </c>
       <c r="E28" s="29">
         <f>IF(Main!D20="Yes",1,0)</f>
@@ -10676,7 +10677,7 @@
       </c>
       <c r="F28" s="38">
         <f t="shared" si="0"/>
-        <v>0.17352000000000001</v>
+        <v>0.12330000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="16.5">
@@ -10689,24 +10690,24 @@
     </row>
     <row r="30" spans="1:6" ht="15.75">
       <c r="A30" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="51">
-        <v>1.1606000000000001</v>
-      </c>
-      <c r="E30" s="29" t="str">
+        <v>25</v>
+      </c>
+      <c r="D30" s="45">
+        <v>1.1608099999999999</v>
+      </c>
+      <c r="E30" s="29">
         <f>IF(Main!D22="Yes",1, IF(Main!D22="No",0,"N/A"))</f>
-        <v>N/A</v>
-      </c>
-      <c r="F30" s="38" t="e">
+        <v>0</v>
+      </c>
+      <c r="F30" s="38">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -10715,7 +10716,7 @@
         <v>7</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31" s="28"/>
       <c r="E31" s="29"/>
@@ -10724,7 +10725,7 @@
     <row r="32" spans="1:6" ht="17.100000000000001" thickBot="1">
       <c r="A32" s="39"/>
       <c r="B32" s="40" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C32" s="44"/>
       <c r="D32" s="41"/>
@@ -10736,86 +10737,86 @@
       <c r="B33" s="14"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="D34" s="50" t="s">
+      <c r="D34" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="50"/>
-      <c r="F34" s="28" t="e">
+      <c r="E34" s="51"/>
+      <c r="F34" s="28">
         <f>SUM(F3,F6,F9,,F12,F15,F18,F21,F24,F27,F30)</f>
-        <v>#VALUE!</v>
+        <v>13.34531</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="D35" s="50" t="s">
+      <c r="D35" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="50"/>
+      <c r="E35" s="51"/>
       <c r="F35" s="28">
         <f>SUM(F4,F7,F10,,F13,F16,F19,F22,F25,F28)</f>
-        <v>11.851910000000002</v>
+        <v>12.76085</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="E36" s="14"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="D37" s="50" t="s">
+      <c r="D37" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="50"/>
-      <c r="F37" s="28" t="e">
-        <f>-16.09924+F34</f>
-        <v>#VALUE!</v>
+      <c r="E37" s="51"/>
+      <c r="F37" s="28">
+        <f>-16.15349+F34</f>
+        <v>-2.8081800000000019</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="D38" s="50" t="s">
+      <c r="D38" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="50"/>
+      <c r="E38" s="51"/>
       <c r="F38" s="28">
-        <f>-15.0531+F35</f>
-        <v>-3.2011899999999986</v>
+        <f>-15.08586+F35</f>
+        <v>-2.3250100000000007</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="D40" s="50" t="s">
+      <c r="D40" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="50"/>
-      <c r="F40" s="28" t="e">
+      <c r="E40" s="51"/>
+      <c r="F40" s="28">
         <f>1/(1+EXP(-(F37)))</f>
-        <v>#VALUE!</v>
+        <v>5.6883741428119E-2</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="D41" s="50" t="s">
+      <c r="D41" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E41" s="50"/>
+      <c r="E41" s="51"/>
       <c r="F41" s="28">
         <f>1/(1+EXP(-(F38)))</f>
-        <v>3.9120965541546253E-2</v>
+        <v>8.9072716344553479E-2</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="D43" s="50" t="s">
+      <c r="D43" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="E43" s="50"/>
-      <c r="F43" s="28" t="e">
+      <c r="E43" s="51"/>
+      <c r="F43" s="28">
         <f>IF(AND(Main!D4&gt;=50,Main!D4 &lt;=73),F40*100,"NA")</f>
-        <v>#VALUE!</v>
+        <v>5.6883741428118997</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="D44" s="50" t="s">
+      <c r="D44" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="E44" s="50"/>
+      <c r="E44" s="51"/>
       <c r="F44" s="28">
         <f>IF(AND(Main!D4&gt;=50,Main!D4 &lt;=73),F41*100,"NA")</f>
-        <v>3.9120965541546253</v>
+        <v>8.9072716344553484</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75"/>

</xml_diff>